<commit_message>
More scrolls. So Scrolly
</commit_message>
<xml_diff>
--- a/src/main/resources/20191202 Positions.xlsx
+++ b/src/main/resources/20191202 Positions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saepiox.sharepoint.com/sites/Saepions/Delte dokumenter/SaepioX Share/11 Test/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\exist\IdeaProjects\atester\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{13E5AC33-8EE0-4DB2-87E9-936006AA9C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{454C889F-CC19-44ED-B45B-3F5481476525}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424CD7D4-1824-4BD9-BDAE-22F35630F0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{78B012A2-6D3E-4E44-BD66-65528F7557E8}"/>
+    <workbookView xWindow="-38145" yWindow="14925" windowWidth="36960" windowHeight="10545" xr2:uid="{78B012A2-6D3E-4E44-BD66-65528F7557E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -324,7 +323,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -333,13 +332,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -363,7 +362,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -401,7 +400,7 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,9 +486,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF00797A-C2E5-4BE8-835D-C2EE130C0357}" name="Table1" displayName="Table1" ref="A1:O51" tableType="xml" totalsRowShown="0">
   <autoFilter ref="A1:O51" xr:uid="{4D6307EA-ED28-41D1-94CF-AAA3D6F6109E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O1">
-    <sortCondition descending="1" ref="N1"/>
-  </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{6D0289A2-702D-4D5B-910C-50404F26EFD8}" uniqueName="PortfolioId" name="PortfolioId">
       <xmlColumnPr mapId="6" xpath="/Positions/Position/PortfolioId" xmlDataType="string"/>
@@ -845,28 +841,28 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
     <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="9" width="19.1328125" customWidth="1"/>
+    <col min="10" max="10" width="31.86328125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="22.40625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.54296875" customWidth="1"/>
+    <col min="15" max="15" width="25.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A2" s="7" t="s">
         <v>49</v>
       </c>
@@ -958,7 +954,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -1004,7 +1000,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A4" s="7" t="s">
         <v>49</v>
       </c>
@@ -1050,7 +1046,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
@@ -1096,7 +1092,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A6" s="7" t="s">
         <v>50</v>
       </c>
@@ -1142,7 +1138,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A7" s="7" t="s">
         <v>50</v>
       </c>
@@ -1188,7 +1184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1231,7 +1227,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1270,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1317,7 +1313,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1360,7 +1356,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1403,7 +1399,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1446,7 +1442,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1488,7 +1484,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1530,7 +1526,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1572,7 +1568,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1614,7 +1610,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1656,7 +1652,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1698,7 +1694,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1740,7 +1736,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1782,7 +1778,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1824,7 +1820,7 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A23" s="7" t="s">
         <v>70</v>
       </c>
@@ -1870,7 +1866,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A24" s="7" t="s">
         <v>70</v>
       </c>
@@ -1916,7 +1912,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A25" s="7" t="s">
         <v>70</v>
       </c>
@@ -1962,7 +1958,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A26" s="7" t="s">
         <v>70</v>
       </c>
@@ -2008,7 +2004,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A27" s="7" t="s">
         <v>49</v>
       </c>
@@ -2053,7 +2049,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A28" s="7" t="s">
         <v>49</v>
       </c>
@@ -2099,7 +2095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A29" s="7" t="s">
         <v>49</v>
       </c>
@@ -2145,7 +2141,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A30" s="7" t="s">
         <v>50</v>
       </c>
@@ -2191,7 +2187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
@@ -2237,7 +2233,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A32" s="7" t="s">
         <v>50</v>
       </c>
@@ -2283,7 +2279,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -2326,7 +2322,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2369,7 +2365,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2412,7 +2408,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -2455,7 +2451,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2498,7 +2494,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -2541,7 +2537,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -2583,7 +2579,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -2625,7 +2621,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -2667,7 +2663,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -2709,7 +2705,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -2751,7 +2747,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -2793,7 +2789,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -2835,7 +2831,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -2877,7 +2873,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -2919,7 +2915,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A48" s="7" t="s">
         <v>70</v>
       </c>
@@ -2965,7 +2961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A49" s="7" t="s">
         <v>70</v>
       </c>
@@ -3011,7 +3007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A50" s="7" t="s">
         <v>70</v>
       </c>
@@ -3057,7 +3053,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A51" s="7" t="s">
         <v>70</v>
       </c>
@@ -3114,21 +3110,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005052ED9CA1DEE4D9762B6CC8CA412A2" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fa1c7641e9ee124d53d5d871ef3c7a5f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44d32ed3-dce8-4c9c-abdf-f5451b0d65e6" xmlns:ns3="75558148-4fda-4f75-a6bf-6c4e67d1b805" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="daf5716be676429fea2c1104adc272bc" ns2:_="" ns3:_="">
     <xsd:import namespace="44d32ed3-dce8-4c9c-abdf-f5451b0d65e6"/>
@@ -3331,10 +3312,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F06A495-283B-46AC-926F-81749FB14875}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C36DE28-70A2-4C05-9039-28FC487A2727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="44d32ed3-dce8-4c9c-abdf-f5451b0d65e6"/>
+    <ds:schemaRef ds:uri="75558148-4fda-4f75-a6bf-6c4e67d1b805"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3357,5 +3364,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C36DE28-70A2-4C05-9039-28FC487A2727}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F06A495-283B-46AC-926F-81749FB14875}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>